<commit_message>
feat: Add task 2
</commit_message>
<xml_diff>
--- a/Problems 2.xlsx
+++ b/Problems 2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t xml:space="preserve">Приведите пример супертипа сущности, не имеющего собственных экземпляров. </t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">Составьте диаграмму прецедентов для своего проекта. Дополните ею документацию.</t>
   </si>
   <si>
+    <t xml:space="preserve">-&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">Маша работает в отделе разработки в Департаменте ИТ, в котором также есть отдел тестирования и отдел поддержки. В компании, где работает Маша всего 4 департамента:</t>
   </si>
   <si>
@@ -67,10 +70,25 @@
     <t xml:space="preserve">Напишите на языке OCL условие того, что водителю не может быть меньше 18 лет. Также напишите условие того, что автомобиль не может быть старше 30 лет.</t>
   </si>
   <si>
+    <t xml:space="preserve">context Водитель inv:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">self.Возраст &gt;= 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">context Автомобиль inv:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">self.Возраст &lt;= 30</t>
+  </si>
+  <si>
     <t xml:space="preserve">Для предыдущей задачи перестройте диаграмму классов так, чтобы можно было написать условие того, что категория ТС должна соответствать категории прав.</t>
   </si>
   <si>
     <t xml:space="preserve">Напишите это условие на OCL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">self.Транспортное средство.категория == self.Права.категория</t>
   </si>
 </sst>
 </file>
@@ -160,16 +178,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,9 +282,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>108360</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>64080</xdr:rowOff>
+      <xdr:rowOff>63720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -272,7 +298,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="611640" y="2750760"/>
-          <a:ext cx="10503720" cy="3647520"/>
+          <a:ext cx="10503360" cy="3647160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -293,9 +319,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>207000</xdr:colOff>
+      <xdr:colOff>206640</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -309,7 +335,192 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="611640" y="6732000"/>
-          <a:ext cx="7544880" cy="3247560"/>
+          <a:ext cx="7544520" cy="3247200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>295920</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>135360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Изображение 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="611640" y="10496520"/>
+          <a:ext cx="8245440" cy="4297680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>137880</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>180360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Изображение 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="611640" y="15382800"/>
+          <a:ext cx="6252840" cy="5428800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>495720</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Изображение 5" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="611640" y="21535920"/>
+          <a:ext cx="10891080" cy="5105520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571680</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Изображение 6" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="611640" y="29679840"/>
+          <a:ext cx="5463720" cy="4142880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>61920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>65880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>268920</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>18000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Изображение 7" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13515120" y="246960"/>
+          <a:ext cx="11825640" cy="16239600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -501,132 +712,561 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:V1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W33" activeCellId="0" sqref="W33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U18" activeCellId="0" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+    </row>
+    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="n">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="B84" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+    </row>
+    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+    </row>
+    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+    </row>
+    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+    </row>
+    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+    </row>
+    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+    </row>
+    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+    </row>
+    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+    </row>
+    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+    </row>
+    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+    </row>
+    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B37" s="0" t="s">
+      <c r="B118" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+    </row>
+    <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+    </row>
+    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+    </row>
+    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+    </row>
+    <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+    </row>
+    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+    </row>
+    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+    </row>
+    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+    </row>
+    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+    </row>
+    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+    </row>
+    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+    </row>
+    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+    </row>
+    <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+    </row>
+    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+    </row>
+    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+    </row>
+    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+    </row>
+    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+    </row>
+    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+    </row>
+    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+    </row>
+    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+    </row>
+    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+    </row>
+    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+    </row>
+    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+    </row>
+    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+    </row>
+    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
+    </row>
+    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B57" s="0" t="s">
+      <c r="B150" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="1"/>
+    </row>
+    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B153" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B154" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="2"/>
+    </row>
+    <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B156" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B157" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B158" s="1"/>
+    </row>
+    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0" t="s">
+      <c r="B159" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B160" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B162" s="2" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B163" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>